<commit_message>
update code luotkham, donthuoc, dangky
</commit_message>
<xml_diff>
--- a/ex.xlsx
+++ b/ex.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>Họ tên</t>
   </si>
@@ -38,184 +38,154 @@
     <t>Ảnh</t>
   </si>
   <si>
+    <t>Nguyen Van A</t>
+  </si>
+  <si>
+    <t>22-02-1980</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>Thach that ha noi</t>
+  </si>
+  <si>
+    <t>09091829334</t>
+  </si>
+  <si>
+    <t>khambenh1@gmail.com</t>
+  </si>
+  <si>
+    <t>http://localhost/ManagerPatientPHP/Public/img/benhnhan1.jpg</t>
+  </si>
+  <si>
+    <t>Nguyen Van B</t>
+  </si>
+  <si>
+    <t>Nữ</t>
+  </si>
+  <si>
+    <t>009812937</t>
+  </si>
+  <si>
+    <t>khambenh2@gmail.com</t>
+  </si>
+  <si>
+    <t>Nguyen Van C</t>
+  </si>
+  <si>
+    <t>08902394732</t>
+  </si>
+  <si>
+    <t>khambenh3@gmail.com</t>
+  </si>
+  <si>
+    <t>Nguyen Van D</t>
+  </si>
+  <si>
+    <t>098298374</t>
+  </si>
+  <si>
+    <t>khambenh4@gmail.com</t>
+  </si>
+  <si>
+    <t>Nguyen Van E</t>
+  </si>
+  <si>
+    <t>09012838734</t>
+  </si>
+  <si>
+    <t>khambenh5@gmail.com</t>
+  </si>
+  <si>
+    <t>http://localhost/ManagerPatientPHP/Public/img/doctor3.jpg</t>
+  </si>
+  <si>
     <t>Nguyen Van F</t>
   </si>
   <si>
-    <t>09-07-1997</t>
-  </si>
-  <si>
-    <t>Nam</t>
+    <t>09012938978</t>
+  </si>
+  <si>
+    <t>khambenh6@gmail.com</t>
+  </si>
+  <si>
+    <t>Nguyen Van G</t>
+  </si>
+  <si>
+    <t>0090192396</t>
+  </si>
+  <si>
+    <t>khambenh7@gmail.com</t>
+  </si>
+  <si>
+    <t>Nguyen Van H</t>
+  </si>
+  <si>
+    <t>0091238987234</t>
+  </si>
+  <si>
+    <t>khambenh8@gmail.com</t>
+  </si>
+  <si>
+    <t>Nguyen Van K</t>
+  </si>
+  <si>
+    <t>0912893947</t>
+  </si>
+  <si>
+    <t>khambenh9@gmail.com</t>
+  </si>
+  <si>
+    <t>Nguyen Van J</t>
+  </si>
+  <si>
+    <t>09018239786</t>
+  </si>
+  <si>
+    <t>khambenh10@gmail.com</t>
+  </si>
+  <si>
+    <t>0901829836876</t>
+  </si>
+  <si>
+    <t>khambenh11@gmail.com</t>
+  </si>
+  <si>
+    <t>Nguyen Van L</t>
+  </si>
+  <si>
+    <t>0019283987</t>
+  </si>
+  <si>
+    <t>khambenh12@gmail.com</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Duy</t>
+  </si>
+  <si>
+    <t>08192873877</t>
+  </si>
+  <si>
+    <t>duykhambenh@gmail.co</t>
+  </si>
+  <si>
+    <t>nguyen van ninh</t>
+  </si>
+  <si>
+    <t>2023-10-10</t>
   </si>
   <si>
     <t>Thach that - ha noi</t>
   </si>
   <si>
-    <t>09012938978</t>
-  </si>
-  <si>
-    <t>khambenh6@gmail.com</t>
-  </si>
-  <si>
-    <t>http://localhost/ManagerPatientPHP/Public/img/benhnhan6.jpg</t>
-  </si>
-  <si>
-    <t>Nguyen Van G</t>
-  </si>
-  <si>
-    <t>17-03-2005</t>
-  </si>
-  <si>
-    <t>0090192396</t>
-  </si>
-  <si>
-    <t>khambenh7@gmail.com</t>
-  </si>
-  <si>
-    <t>http://localhost/ManagerPatientPHP/Public/img/benhnhan1.jpg</t>
-  </si>
-  <si>
-    <t>Nguyen Van H</t>
-  </si>
-  <si>
-    <t>13-03-1997</t>
-  </si>
-  <si>
-    <t>0091238987234</t>
-  </si>
-  <si>
-    <t>khambenh8@gmail.com</t>
+    <t>0456321312</t>
+  </si>
+  <si>
+    <t>bankankis@gmail.com</t>
   </si>
   <si>
     <t>http://localhost/ManagerPatientPHP/Public/img/benhnhan4.jpg</t>
-  </si>
-  <si>
-    <t>Nguyen Van K</t>
-  </si>
-  <si>
-    <t>13-03-1998</t>
-  </si>
-  <si>
-    <t>0912893947</t>
-  </si>
-  <si>
-    <t>khambenh9@gmail.com</t>
-  </si>
-  <si>
-    <t>http://localhost/ManagerPatientPHP/Public/img/benhnhan5.jpg</t>
-  </si>
-  <si>
-    <t>Nguyen Van J</t>
-  </si>
-  <si>
-    <t>18-03-1999</t>
-  </si>
-  <si>
-    <t>Nữ</t>
-  </si>
-  <si>
-    <t>09018239786</t>
-  </si>
-  <si>
-    <t>khambenh10@gmail.com</t>
-  </si>
-  <si>
-    <t>http://localhost/ManagerPatientPHP/Public/img/benhnhan2.jpg</t>
-  </si>
-  <si>
-    <t>08-03-1995</t>
-  </si>
-  <si>
-    <t>0901829836876</t>
-  </si>
-  <si>
-    <t>khambenh11@gmail.com</t>
-  </si>
-  <si>
-    <t>Nguyen Van L</t>
-  </si>
-  <si>
-    <t>08-07-1999</t>
-  </si>
-  <si>
-    <t>0019283987</t>
-  </si>
-  <si>
-    <t>khambenh12@gmail.com</t>
-  </si>
-  <si>
-    <t>Nguyen Van A</t>
-  </si>
-  <si>
-    <t>22-06-2000</t>
-  </si>
-  <si>
-    <t>Thach That - Ha Noi</t>
-  </si>
-  <si>
-    <t>09091829334</t>
-  </si>
-  <si>
-    <t>khambenh1@gmail.com</t>
-  </si>
-  <si>
-    <t>https://cdn.tgdd.vn/Files/2016/02/25/792452/chup-anh-hoang-hon-bang-smartphone_800x450.jpg</t>
-  </si>
-  <si>
-    <t>Nguyen Van B</t>
-  </si>
-  <si>
-    <t>13-07-2000</t>
-  </si>
-  <si>
-    <t>009812937</t>
-  </si>
-  <si>
-    <t>khambenh2@gmail.com</t>
-  </si>
-  <si>
-    <t>Nguyen Van D</t>
-  </si>
-  <si>
-    <t>098298374</t>
-  </si>
-  <si>
-    <t>khambenh4@gmail.com</t>
-  </si>
-  <si>
-    <t>Nguyen Van C</t>
-  </si>
-  <si>
-    <t>29-01-2003</t>
-  </si>
-  <si>
-    <t>08902394732</t>
-  </si>
-  <si>
-    <t>khambenh3@gmail.com</t>
-  </si>
-  <si>
-    <t>06-02-1997</t>
-  </si>
-  <si>
-    <t>0098765432</t>
-  </si>
-  <si>
-    <t>phongkham2@gmail.com</t>
-  </si>
-  <si>
-    <t>Nguyen Van E</t>
-  </si>
-  <si>
-    <t>06-09-2023</t>
-  </si>
-  <si>
-    <t>09012838734</t>
-  </si>
-  <si>
-    <t>khambenh5@gmail.com</t>
-  </si>
-  <si>
-    <t>http://localhost/ManagerPatientPHP/Public/img/benhnhan3.jpg</t>
   </si>
 </sst>
 </file>
@@ -554,7 +524,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -613,10 +583,10 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -628,119 +598,119 @@
         <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
         <v>13</v>
@@ -748,68 +718,68 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="G11" t="s">
         <v>13</v>
@@ -817,71 +787,94 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="F14" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G14" t="s">
-        <v>66</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>